<commit_message>
Just finished the Email automation course
</commit_message>
<xml_diff>
--- a/2. Automation Developer Associate/7. Error and Exception Handling/Try Catch/Practice1.xlsx
+++ b/2. Automation Developer Associate/7. Error and Exception Handling/Try Catch/Practice1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20405"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F2944DC-2933-47DF-B0AA-BDA1B8922391}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED5EEC8-930D-4CFF-90DC-3DE0C2E6D143}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22935" yWindow="-105" windowWidth="30930" windowHeight="16890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="22935" yWindow="-105" windowWidth="30930" windowHeight="16890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CashFlow" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="23">
   <si>
     <t>Month</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t>22K</t>
+  </si>
+  <si>
+    <t>ERROR</t>
+  </si>
+  <si>
+    <t>SUCCESS</t>
   </si>
 </sst>
 </file>
@@ -448,7 +454,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -489,6 +495,9 @@
       <c r="D2">
         <v>226</v>
       </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
@@ -503,6 +512,9 @@
       <c r="D3">
         <v>13</v>
       </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
@@ -517,6 +529,9 @@
       <c r="D4">
         <v>-20</v>
       </c>
+      <c r="E4" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
@@ -529,7 +544,10 @@
         <v>130</v>
       </c>
       <c r="D5">
-        <v>-66</v>
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -543,7 +561,10 @@
         <v>78</v>
       </c>
       <c r="D6">
-        <v>16</v>
+        <v>-66</v>
+      </c>
+      <c r="E6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -557,7 +578,10 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>35</v>
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -571,7 +595,10 @@
         <v>13</v>
       </c>
       <c r="D8">
-        <v>42</v>
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -585,7 +612,10 @@
         <v>49</v>
       </c>
       <c r="D9">
-        <v>-16</v>
+        <v>16</v>
+      </c>
+      <c r="E9" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -599,7 +629,10 @@
         <v>169</v>
       </c>
       <c r="D10">
-        <v>-31</v>
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -613,7 +646,10 @@
         <v>9</v>
       </c>
       <c r="D11">
-        <v>-16</v>
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -627,7 +663,10 @@
         <v>91</v>
       </c>
       <c r="D12">
-        <v>-104</v>
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -641,7 +680,10 @@
         <v>7</v>
       </c>
       <c r="D13">
-        <v>13</v>
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -655,7 +697,10 @@
         <v>37</v>
       </c>
       <c r="D14">
-        <v>-115</v>
+        <v>-16</v>
+      </c>
+      <c r="E14" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -669,7 +714,10 @@
         <v>123</v>
       </c>
       <c r="D15">
-        <v>-29</v>
+        <v>-31</v>
+      </c>
+      <c r="E15" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -683,10 +731,13 @@
         <v>73</v>
       </c>
       <c r="D16">
-        <v>-14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-16</v>
+      </c>
+      <c r="E16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>42583</v>
       </c>
@@ -697,10 +748,13 @@
         <v>39</v>
       </c>
       <c r="D17">
-        <v>-10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-104</v>
+      </c>
+      <c r="E17" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>42614</v>
       </c>
@@ -711,10 +765,13 @@
         <v>11</v>
       </c>
       <c r="D18">
-        <v>-79</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>42644</v>
       </c>
@@ -725,10 +782,13 @@
         <v>35</v>
       </c>
       <c r="D19">
-        <v>-142</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>42675</v>
       </c>
@@ -739,10 +799,13 @@
         <v>12</v>
       </c>
       <c r="D20">
-        <v>-40</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>42705</v>
       </c>
@@ -753,10 +816,13 @@
         <v>45</v>
       </c>
       <c r="D21">
-        <v>-41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-115</v>
+      </c>
+      <c r="E21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>42736</v>
       </c>
@@ -767,10 +833,13 @@
         <v>13</v>
       </c>
       <c r="D22">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>42767</v>
       </c>
@@ -781,10 +850,13 @@
         <v>15</v>
       </c>
       <c r="D23">
-        <v>-93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>42795</v>
       </c>
@@ -795,10 +867,13 @@
         <v>14</v>
       </c>
       <c r="D24">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>42826</v>
       </c>
@@ -809,10 +884,13 @@
         <v>21</v>
       </c>
       <c r="D25">
-        <v>-43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>42856</v>
       </c>
@@ -823,10 +901,13 @@
         <v>12</v>
       </c>
       <c r="D26">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-10</v>
+      </c>
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>42887</v>
       </c>
@@ -837,10 +918,13 @@
         <v>55</v>
       </c>
       <c r="D27">
-        <v>-118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-79</v>
+      </c>
+      <c r="E27" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>42917</v>
       </c>
@@ -851,10 +935,13 @@
         <v>87</v>
       </c>
       <c r="D28">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-142</v>
+      </c>
+      <c r="E28" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>42948</v>
       </c>
@@ -865,10 +952,13 @@
         <v>33</v>
       </c>
       <c r="D29">
-        <v>-64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-40</v>
+      </c>
+      <c r="E29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>42979</v>
       </c>
@@ -879,10 +969,13 @@
         <v>89</v>
       </c>
       <c r="D30">
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>43009</v>
       </c>
@@ -893,10 +986,13 @@
         <v>14</v>
       </c>
       <c r="D31">
-        <v>-26</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-41</v>
+      </c>
+      <c r="E31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>43040</v>
       </c>
@@ -907,10 +1003,13 @@
         <v>15</v>
       </c>
       <c r="D32">
-        <v>-36</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>43070</v>
       </c>
@@ -921,10 +1020,13 @@
         <v>22</v>
       </c>
       <c r="D33">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="E33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>43101</v>
       </c>
@@ -934,8 +1036,14 @@
       <c r="C34" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>-93</v>
+      </c>
+      <c r="E34" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>43132</v>
       </c>
@@ -945,8 +1053,14 @@
       <c r="C35" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>43160</v>
       </c>
@@ -956,8 +1070,14 @@
       <c r="C36" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>43191</v>
       </c>
@@ -967,8 +1087,14 @@
       <c r="C37" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>43221</v>
       </c>
@@ -978,8 +1104,14 @@
       <c r="C38" s="3">
         <v>34</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D38">
+        <v>20</v>
+      </c>
+      <c r="E38" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>43252</v>
       </c>
@@ -989,8 +1121,14 @@
       <c r="C39" s="3">
         <v>14</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D39">
+        <v>-43</v>
+      </c>
+      <c r="E39" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>43282</v>
       </c>
@@ -1000,8 +1138,14 @@
       <c r="C40" s="3">
         <v>55</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D40">
+        <v>41</v>
+      </c>
+      <c r="E40" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>43313</v>
       </c>
@@ -1011,8 +1155,14 @@
       <c r="C41" s="3">
         <v>44</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>43344</v>
       </c>
@@ -1022,8 +1172,14 @@
       <c r="C42" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D42">
+        <v>-118</v>
+      </c>
+      <c r="E42" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>43374</v>
       </c>
@@ -1033,8 +1189,14 @@
       <c r="C43" s="3">
         <v>16</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43405</v>
       </c>
@@ -1044,8 +1206,14 @@
       <c r="C44" s="3">
         <v>77</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D44">
+        <v>32</v>
+      </c>
+      <c r="E44" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>43435</v>
       </c>
@@ -1055,8 +1223,14 @@
       <c r="C45" s="3">
         <v>24</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D45">
+        <v>-64</v>
+      </c>
+      <c r="E45" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>43466</v>
       </c>
@@ -1066,8 +1240,14 @@
       <c r="C46" s="3">
         <v>12</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D46">
+        <v>-2</v>
+      </c>
+      <c r="E46" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>43497</v>
       </c>
@@ -1077,8 +1257,14 @@
       <c r="C47" s="3">
         <v>18</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D47">
+        <v>-26</v>
+      </c>
+      <c r="E47" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>43525</v>
       </c>
@@ -1088,8 +1274,14 @@
       <c r="C48" s="3">
         <v>19</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D48">
+        <v>-36</v>
+      </c>
+      <c r="E48" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>43556</v>
       </c>
@@ -1099,8 +1291,14 @@
       <c r="C49" s="3" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>43586</v>
       </c>
@@ -1110,8 +1308,14 @@
       <c r="C50" s="3">
         <v>87</v>
       </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D50">
+        <v>54</v>
+      </c>
+      <c r="E50" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
     </row>
   </sheetData>

</xml_diff>